<commit_message>
ready for pandas 2.0
</commit_message>
<xml_diff>
--- a/jupyter/data/df0.xlsx
+++ b/jupyter/data/df0.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,21 +470,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Maja</t>
+          <t>Susanne</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>25143</v>
+        <v>27701</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>teQDdÜl5</t>
+          <t>jDÖRöm</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -494,21 +494,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Albert</t>
+          <t>Edith</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="C3" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>42913</v>
+        <v>15624</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>üB0JLnyfld</t>
+          <t>uCuNiXyrXH</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -518,21 +518,21 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kim</t>
+          <t>Sebastian</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C4" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D4" t="n">
-        <v>10956</v>
+        <v>12687</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>änuR1</t>
+          <t>udyFEOnLwd</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -542,21 +542,21 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Carolin</t>
+          <t>Nikolas</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C5" t="n">
         <v>30</v>
       </c>
       <c r="D5" t="n">
-        <v>14876</v>
+        <v>95722</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>57näy9PA</t>
+          <t>ZäiixM</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -566,21 +566,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Jan</t>
+          <t>Mathias</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C6" t="n">
         <v>30</v>
       </c>
       <c r="D6" t="n">
-        <v>13248</v>
+        <v>10916</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>MkQiöBg8WK</t>
+          <t>aSwceOWySD</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -590,21 +590,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Anna</t>
+          <t>Jakob</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" t="n">
         <v>30</v>
       </c>
       <c r="D7" t="n">
-        <v>29700</v>
+        <v>33759</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>6Kr0d2oj</t>
+          <t>8EauRvU8I</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -614,21 +614,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Sebastian</t>
+          <t>Till</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C8" t="n">
         <v>30</v>
       </c>
       <c r="D8" t="n">
-        <v>84835</v>
+        <v>95121</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>üUL2ER</t>
+          <t>Ä4iMUD</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -638,21 +638,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Amelie</t>
+          <t>Swen</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="C9" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D9" t="n">
-        <v>56644</v>
+        <v>99782</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>qpjNHws</t>
+          <t>rIXäx</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -662,21 +662,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Carina</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C10" t="n">
         <v>20</v>
       </c>
       <c r="D10" t="n">
-        <v>91402</v>
+        <v>89005</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>IPRicl0su</t>
+          <t>i59c6z7</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -686,21 +686,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Arne</t>
+          <t>Ayleen</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C11" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>49287</v>
+        <v>59290</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>cq2Ah72</t>
+          <t>bZRÄühni</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -710,21 +710,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Lennard</t>
+          <t>Merle</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="C12" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>82867</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>LWfrÄ3</t>
+          <t>pJpLUü2duA</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -734,21 +734,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Hannes</t>
+          <t>Gertrud</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" t="n">
         <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>46592</v>
+        <v>15563</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Db0üÜI</t>
+          <t>Yn8zpUIzE</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -758,21 +758,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Nadine</t>
+          <t>Johann</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C14" t="n">
         <v>30</v>
       </c>
       <c r="D14" t="n">
-        <v>32989</v>
+        <v>85033</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>yaj1q</t>
+          <t>2Ra02vyoIS</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -782,21 +782,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Ulrike</t>
+          <t>Isabella</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D15" t="n">
-        <v>55404</v>
+        <v>96557</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>9QD3m1dt</t>
+          <t>MLn9u0LV</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -806,21 +806,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Brigitte</t>
+          <t>Christiane</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C16" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D16" t="n">
-        <v>11442</v>
+        <v>36071</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Idi6Ä</t>
+          <t>VuITuZbY</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -830,21 +830,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Fynn</t>
+          <t>Rosemarie</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C17" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D17" t="n">
-        <v>22211</v>
+        <v>68057</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>RiO5M4</t>
+          <t>0BPZQk</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -854,21 +854,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Marius</t>
+          <t>Yannik</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C18" t="n">
         <v>20</v>
       </c>
       <c r="D18" t="n">
-        <v>38655</v>
+        <v>43600</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>24xFWb0Ü</t>
+          <t>Je6s7O</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -878,21 +878,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Heike</t>
+          <t>Thorsten</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C19" t="n">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="D19" t="n">
-        <v>85467</v>
+        <v>19988</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>fpÜwR</t>
+          <t>xpePöb</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -902,21 +902,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Niclas</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C20" t="n">
         <v>30</v>
       </c>
       <c r="D20" t="n">
-        <v>68610</v>
+        <v>68999</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>qÖwtr8ly</t>
+          <t>O5ÄLJj</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -926,21 +926,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Stephan</t>
+          <t>Ole</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="C21" t="n">
         <v>30</v>
       </c>
       <c r="D21" t="n">
-        <v>40103</v>
+        <v>43700</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>NPYocuLbf</t>
+          <t>b9ICqlG2</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -950,21 +950,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Dagmar</t>
+          <t>Luis</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C22" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D22" t="n">
-        <v>20919</v>
+        <v>37592</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>RetKH</t>
+          <t>YT9hIVfj</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -974,21 +974,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Rene</t>
+          <t>Erika</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C23" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D23" t="n">
-        <v>99802</v>
+        <v>12727</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>2jTIAAq</t>
+          <t>SKbväaöZD</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -998,21 +998,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Carla</t>
+          <t>Sylvia</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C24" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D24" t="n">
-        <v>84491</v>
+        <v>86657</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>uxaSOC</t>
+          <t>NvbVufd</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1022,21 +1022,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Stephan</t>
+          <t>Adrian</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C25" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D25" t="n">
-        <v>25143</v>
+        <v>56789</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>staB8cKag9</t>
+          <t>Uojte</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1046,21 +1046,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Dagmar</t>
+          <t>Carolin</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C26" t="n">
         <v>20</v>
       </c>
       <c r="D26" t="n">
-        <v>30075</v>
+        <v>21048</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>ÖojLm</t>
+          <t>YCöveRcvD</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1070,21 +1070,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Katja</t>
+          <t>Gisela</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C27" t="n">
         <v>30</v>
       </c>
       <c r="D27" t="n">
-        <v>29700</v>
+        <v>84942</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>äBEöRVahDV</t>
+          <t>joyeXPwM</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -1094,21 +1094,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Miriam</t>
+          <t>Cornelia</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="C28" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D28" t="n">
-        <v>80630</v>
+        <v>49860</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>DbTsifs</t>
+          <t>S9rMmgKH7</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -1118,21 +1118,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Annette</t>
+          <t>Willy</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="C29" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D29" t="n">
-        <v>41162</v>
+        <v>97729</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>qGma6eUyP</t>
+          <t>nrj3w</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -1142,21 +1142,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Fynn</t>
+          <t>Nathalie</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="C30" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D30" t="n">
-        <v>13504</v>
+        <v>64481</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>4öXnjföauT</t>
+          <t>HyZGYZKjl9</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -1166,21 +1166,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Fynn</t>
+          <t>Christiane</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C31" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D31" t="n">
-        <v>97069</v>
+        <v>99288</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>6oy6heV</t>
+          <t>Gwd4Ü</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -1190,21 +1190,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Fynn</t>
+          <t>Claus</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C32" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D32" t="n">
-        <v>38453</v>
+        <v>49860</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>GSQöäPaimp</t>
+          <t>oVb8msT</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -1214,21 +1214,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Richard</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C33" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D33" t="n">
-        <v>71929</v>
+        <v>36071</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>26xZBf</t>
+          <t>84tmGz</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -1238,21 +1238,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Heike</t>
+          <t>Sebastian</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C34" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D34" t="n">
-        <v>99802</v>
+        <v>53782</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>67eeKÖR2</t>
+          <t>RoÖÖoVGÄ</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -1262,7 +1262,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Carla</t>
+          <t>Johann</t>
         </is>
       </c>
       <c r="B35" t="n">
@@ -1272,62 +1272,14 @@
         <v>30</v>
       </c>
       <c r="D35" t="n">
-        <v>33759</v>
+        <v>45315</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>f6zB1JLSf</t>
+          <t>caüFa</t>
         </is>
       </c>
       <c r="F35" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Niclas</t>
-        </is>
-      </c>
-      <c r="B36" t="n">
-        <v>31</v>
-      </c>
-      <c r="C36" t="n">
-        <v>30</v>
-      </c>
-      <c r="D36" t="n">
-        <v>45905</v>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>ROh0GgoO</t>
-        </is>
-      </c>
-      <c r="F36" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Brigitte</t>
-        </is>
-      </c>
-      <c r="B37" t="n">
-        <v>32</v>
-      </c>
-      <c r="C37" t="n">
-        <v>30</v>
-      </c>
-      <c r="D37" t="n">
-        <v>0</v>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Ivuvwe</t>
-        </is>
-      </c>
-      <c r="F37" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1342,7 +1294,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1385,21 +1337,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Annette</t>
+          <t>Amelie</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D2" t="n">
-        <v>77261</v>
+        <v>60544</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>bGz432sÜY4</t>
+          <t>iuueq0Fvo</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -1409,21 +1361,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Waltraud</t>
+          <t>Jannis</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C3" t="n">
         <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>93731</v>
+        <v>10704</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>O418DA63</t>
+          <t>5VRqG</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -1433,21 +1385,21 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Adrian</t>
+          <t>Linda</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C4" t="n">
         <v>30</v>
       </c>
       <c r="D4" t="n">
-        <v>11227</v>
+        <v>45315</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>ziigaüfAra</t>
+          <t>kHf1eaÄLR</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -1457,21 +1409,21 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Birgit</t>
+          <t>Niko</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C5" t="n">
         <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>38437</v>
+        <v>59707</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>ÜYuzWu</t>
+          <t>ü9EHnG0Äo</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -1481,21 +1433,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Vincent</t>
+          <t>Claus</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C6" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D6" t="n">
-        <v>72636</v>
+        <v>65053</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>H0XBab</t>
+          <t>Ö2rSon4v</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -1505,21 +1457,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Beate</t>
+          <t>Anja</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C7" t="n">
         <v>30</v>
       </c>
       <c r="D7" t="n">
-        <v>86126</v>
+        <v>11575</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>op8uu</t>
+          <t>hdwS5</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -1529,21 +1481,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>David</t>
+          <t>Kevin</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D8" t="n">
-        <v>82232</v>
+        <v>90714</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>oDeue</t>
+          <t>ndjIoua5</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -1553,21 +1505,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Adolf</t>
+          <t>Else</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C9" t="n">
         <v>20</v>
       </c>
       <c r="D9" t="n">
-        <v>35203</v>
+        <v>38213</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Wolq6</t>
+          <t>yRRÖooH</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -1577,21 +1529,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Till</t>
+          <t>Vincent</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" t="n">
         <v>20</v>
       </c>
       <c r="D10" t="n">
-        <v>37498</v>
+        <v>23736</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>RfZHfV7</t>
+          <t>BtMZh2</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -1601,21 +1553,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Bruno</t>
+          <t>Tom</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="C11" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>63450</v>
+        <v>95150</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>dc4g8g9ON</t>
+          <t>1EzW90D0</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -1625,21 +1577,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tom</t>
+          <t>Astrid</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C12" t="n">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D12" t="n">
-        <v>31138</v>
+        <v>18029</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>z5denuH</t>
+          <t>Ü9AÜjPN</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -1649,21 +1601,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Philip</t>
+          <t>Marius</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C13" t="n">
         <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>64716</v>
+        <v>50902</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>NOoeüHäwHP</t>
+          <t>OcjGui</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -1673,21 +1625,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Nikolas</t>
+          <t>Volker</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C14" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D14" t="n">
-        <v>38453</v>
+        <v>81822</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>l3ZudgW</t>
+          <t>FnMFitQü5</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -1697,21 +1649,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Jürgen</t>
+          <t>Josefine</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D15" t="n">
-        <v>55981</v>
+        <v>61808</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>öP5äz82PÖ9</t>
+          <t>YiPuaKcGfx</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -1721,21 +1673,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Hermann</t>
+          <t>Luca</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C16" t="n">
         <v>30</v>
       </c>
       <c r="D16" t="n">
-        <v>32192</v>
+        <v>24578</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>RäBsHIeMly</t>
+          <t>S73luY87</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -1745,21 +1697,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Elli</t>
+          <t>Oliver</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C17" t="n">
         <v>30</v>
       </c>
       <c r="D17" t="n">
-        <v>80176</v>
+        <v>40378</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>DozUmc</t>
+          <t>nw3kJ5VNf</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -1769,21 +1721,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Stephanie</t>
+          <t>Tanja</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="C18" t="n">
         <v>30</v>
       </c>
       <c r="D18" t="n">
-        <v>67923</v>
+        <v>53782</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>PPNöfK7nö</t>
+          <t>SPidJ</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -1793,21 +1745,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Carla</t>
+          <t>Ilse</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="C19" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D19" t="n">
-        <v>30200</v>
+        <v>86225</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>öskQFnrÜY</t>
+          <t>eÖJxIz6</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -1817,21 +1769,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Werner</t>
+          <t>Vivien</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C20" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D20" t="n">
-        <v>80630</v>
+        <v>69603</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>SK5uaSA</t>
+          <t>iQrhxDwjn</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -1841,21 +1793,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Franz</t>
+          <t>Caroline</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" t="n">
         <v>20</v>
       </c>
       <c r="D21" t="n">
-        <v>81488</v>
+        <v>24559</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>ÄÖxJGE</t>
+          <t>w8uSwlJ4R</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -1865,21 +1817,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Luis</t>
+          <t>Nico</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C22" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D22" t="n">
-        <v>17343</v>
+        <v>36999</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>AeälOJjLH</t>
+          <t>AW4AGu</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -1889,21 +1841,21 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Monika</t>
+          <t>Moritz</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C23" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D23" t="n">
-        <v>0</v>
+        <v>38577</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>e7Ni4</t>
+          <t>YFJ0Udo</t>
         </is>
       </c>
       <c r="F23" t="n">
@@ -1913,21 +1865,21 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Marko</t>
+          <t>Elli</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C24" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D24" t="n">
-        <v>56665</v>
+        <v>0</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>ALS1C7a</t>
+          <t>Moa3GBä</t>
         </is>
       </c>
       <c r="F24" t="n">
@@ -1937,21 +1889,21 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Louise</t>
+          <t>Phillip</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C25" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D25" t="n">
-        <v>44582</v>
+        <v>36755</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>vl9V0XUai</t>
+          <t>3DfiÖgÜO</t>
         </is>
       </c>
       <c r="F25" t="n">
@@ -1961,21 +1913,21 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Sofie</t>
+          <t>Ingo</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C26" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D26" t="n">
-        <v>89620</v>
+        <v>20721</v>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>JiuDl2</t>
+          <t>43nehu</t>
         </is>
       </c>
       <c r="F26" t="n">
@@ -1985,21 +1937,21 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Lisa</t>
+          <t>Bärbel</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C27" t="n">
         <v>20</v>
       </c>
       <c r="D27" t="n">
-        <v>53513</v>
+        <v>38213</v>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>2DwcapYlk</t>
+          <t>50axQll</t>
         </is>
       </c>
       <c r="F27" t="n">
@@ -2009,21 +1961,21 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Denis</t>
+          <t>Sebastian</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C28" t="n">
         <v>30</v>
       </c>
       <c r="D28" t="n">
-        <v>36892</v>
+        <v>68999</v>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>1ezäjp</t>
+          <t>rnbPGGrAv</t>
         </is>
       </c>
       <c r="F28" t="n">
@@ -2033,21 +1985,21 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Katja</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C29" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D29" t="n">
-        <v>46487</v>
+        <v>80786</v>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>ZNWTiuwIV</t>
+          <t>fiviP</t>
         </is>
       </c>
       <c r="F29" t="n">
@@ -2057,21 +2009,21 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Dominik</t>
+          <t>Gertrud</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="C30" t="n">
         <v>30</v>
       </c>
       <c r="D30" t="n">
-        <v>97069</v>
+        <v>23736</v>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>cJKHW</t>
+          <t>56ÜXwä2</t>
         </is>
       </c>
       <c r="F30" t="n">
@@ -2081,21 +2033,21 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Nikolas</t>
+          <t>Kim</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="C31" t="n">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="D31" t="n">
-        <v>18575</v>
+        <v>95150</v>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>eyxqÖülT</t>
+          <t>7ÄMefDÄÄ</t>
         </is>
       </c>
       <c r="F31" t="n">
@@ -2105,21 +2057,21 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Lennard</t>
+          <t>Hertha</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C32" t="n">
         <v>20</v>
       </c>
       <c r="D32" t="n">
-        <v>32989</v>
+        <v>59290</v>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>ShZqzmAZA</t>
+          <t>Öcr1ÖHaUi</t>
         </is>
       </c>
       <c r="F32" t="n">
@@ -2129,21 +2081,21 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Heike</t>
+          <t>Erika</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="C33" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D33" t="n">
-        <v>38437</v>
+        <v>24578</v>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>jrXZn4GCU</t>
+          <t>dK9aq</t>
         </is>
       </c>
       <c r="F33" t="n">
@@ -2153,21 +2105,21 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Rene</t>
+          <t>Hertha</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="C34" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D34" t="n">
-        <v>78155</v>
+        <v>24559</v>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>3Gj0hwQE</t>
+          <t>F6CNohV</t>
         </is>
       </c>
       <c r="F34" t="n">
@@ -2177,21 +2129,21 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Albert</t>
+          <t>Yannic</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C35" t="n">
         <v>20</v>
       </c>
       <c r="D35" t="n">
-        <v>0</v>
+        <v>86328</v>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>äPqABvg</t>
+          <t>OKIaLpxai</t>
         </is>
       </c>
       <c r="F35" t="n">
@@ -2201,21 +2153,21 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Adrian</t>
+          <t>Georg</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="C36" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D36" t="n">
-        <v>31256</v>
+        <v>0</v>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>ameL2</t>
+          <t>TÄnMöQZKr</t>
         </is>
       </c>
       <c r="F36" t="n">
@@ -2225,21 +2177,21 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Simon</t>
+          <t>Yannik</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C37" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D37" t="n">
-        <v>46487</v>
+        <v>56789</v>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>O0Xusäw</t>
+          <t>Gäuz8ÖLo</t>
         </is>
       </c>
       <c r="F37" t="n">
@@ -2249,24 +2201,192 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Arne</t>
+          <t>Lisa</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C38" t="n">
         <v>30</v>
       </c>
       <c r="D38" t="n">
-        <v>55404</v>
+        <v>15563</v>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>GNarZRBkMX</t>
+          <t>L7elwQ</t>
         </is>
       </c>
       <c r="F38" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Mathias</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>36</v>
+      </c>
+      <c r="C39" t="n">
+        <v>30</v>
+      </c>
+      <c r="D39" t="n">
+        <v>84942</v>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>o2tsYHOh</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Ilse</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>35</v>
+      </c>
+      <c r="C40" t="n">
+        <v>30</v>
+      </c>
+      <c r="D40" t="n">
+        <v>15624</v>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>xdö3qu1aGC</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Jakob</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>36</v>
+      </c>
+      <c r="C41" t="n">
+        <v>30</v>
+      </c>
+      <c r="D41" t="n">
+        <v>27701</v>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Q9OUzpeB3N</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Willy</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>30</v>
+      </c>
+      <c r="C42" t="n">
+        <v>30</v>
+      </c>
+      <c r="D42" t="n">
+        <v>43700</v>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>JHYöaVK</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Nikolas</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>38</v>
+      </c>
+      <c r="C43" t="n">
+        <v>30</v>
+      </c>
+      <c r="D43" t="n">
+        <v>89005</v>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>JOb9BNT</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Luis</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>24</v>
+      </c>
+      <c r="C44" t="n">
+        <v>20</v>
+      </c>
+      <c r="D44" t="n">
+        <v>38577</v>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>0WgikeZG</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Rudolph</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>29</v>
+      </c>
+      <c r="C45" t="n">
+        <v>20</v>
+      </c>
+      <c r="D45" t="n">
+        <v>10748</v>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>öNOYjP91Ho</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
         <v>1</v>
       </c>
     </row>
@@ -2281,7 +2401,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2324,21 +2444,21 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Lilli</t>
+          <t>Kurt</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D2" t="n">
-        <v>73588</v>
+        <v>94506</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>oCkaAX70v</t>
+          <t>vpGGs</t>
         </is>
       </c>
       <c r="F2" t="n">
@@ -2348,21 +2468,21 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Rainer</t>
+          <t>Rudolph</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C3" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D3" t="n">
-        <v>81548</v>
+        <v>10748</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>ürqVpbf</t>
+          <t>SÜJoC7j</t>
         </is>
       </c>
       <c r="F3" t="n">
@@ -2372,21 +2492,21 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Anja</t>
+          <t>Anna</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C4" t="n">
         <v>30</v>
       </c>
       <c r="D4" t="n">
-        <v>94972</v>
+        <v>99288</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>dgTv5f3r</t>
+          <t>üV9yu</t>
         </is>
       </c>
       <c r="F4" t="n">
@@ -2396,21 +2516,21 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Matthias</t>
+          <t>Carina</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="C5" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D5" t="n">
-        <v>69967</v>
+        <v>31099</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>VismI4uÄ</t>
+          <t>LcZUb</t>
         </is>
       </c>
       <c r="F5" t="n">
@@ -2420,21 +2540,21 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Johannes</t>
+          <t>Hertha</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C6" t="n">
         <v>30</v>
       </c>
       <c r="D6" t="n">
-        <v>84632</v>
+        <v>77374</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>VQUqigFRÖs</t>
+          <t>OtwSFb2BP</t>
         </is>
       </c>
       <c r="F6" t="n">
@@ -2444,21 +2564,21 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Miriam</t>
+          <t>Bärbel</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D7" t="n">
-        <v>33759</v>
+        <v>80786</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>ZsÖsücip</t>
+          <t>RAoeD1äWn</t>
         </is>
       </c>
       <c r="F7" t="n">
@@ -2468,21 +2588,21 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Richard</t>
+          <t>Paul</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="C8" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D8" t="n">
-        <v>18575</v>
+        <v>0</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>U0JSCd7F3</t>
+          <t>DrQJaRKÜu</t>
         </is>
       </c>
       <c r="F8" t="n">
@@ -2492,21 +2612,21 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Günther</t>
+          <t>Georg</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" t="n">
         <v>30</v>
       </c>
       <c r="D9" t="n">
-        <v>82006</v>
+        <v>90731</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>ÄtÖmUüÜÄC</t>
+          <t>QiaKÖis</t>
         </is>
       </c>
       <c r="F9" t="n">
@@ -2516,21 +2636,21 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Luka</t>
+          <t>Anke</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="C10" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D10" t="n">
-        <v>45905</v>
+        <v>41876</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>9an5öÄ1</t>
+          <t>wunÄluRM1I</t>
         </is>
       </c>
       <c r="F10" t="n">
@@ -2540,21 +2660,21 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Jannis</t>
+          <t>Martha</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="C11" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D11" t="n">
-        <v>84491</v>
+        <v>44825</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Xog14Ätc</t>
+          <t>osLnc</t>
         </is>
       </c>
       <c r="F11" t="n">
@@ -2564,21 +2684,21 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Tina</t>
+          <t>Kathrin</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C12" t="n">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="D12" t="n">
-        <v>71929</v>
+        <v>86328</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>AAAfH</t>
+          <t>ärLVqYKu</t>
         </is>
       </c>
       <c r="F12" t="n">
@@ -2588,21 +2708,21 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Simon</t>
+          <t>Walter</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="C13" t="n">
         <v>30</v>
       </c>
       <c r="D13" t="n">
-        <v>39516</v>
+        <v>45747</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>boxhVE6</t>
+          <t>BRCmme</t>
         </is>
       </c>
       <c r="F13" t="n">
@@ -2612,21 +2732,21 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Oliver</t>
+          <t>Ulrich</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C14" t="n">
         <v>20</v>
       </c>
       <c r="D14" t="n">
-        <v>31256</v>
+        <v>51727</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>yyLDaogQö</t>
+          <t>dosvtsÄoV</t>
         </is>
       </c>
       <c r="F14" t="n">
@@ -2636,21 +2756,21 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Natalie</t>
+          <t>Berndt</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="C15" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D15" t="n">
-        <v>14920</v>
+        <v>0</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>äJy64e</t>
+          <t>laIUti</t>
         </is>
       </c>
       <c r="F15" t="n">
@@ -2660,21 +2780,21 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Jule</t>
+          <t>Lara</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C16" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D16" t="n">
-        <v>81292</v>
+        <v>17098</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>vDB0yiDC</t>
+          <t>ZRa3aLCL</t>
         </is>
       </c>
       <c r="F16" t="n">
@@ -2684,21 +2804,21 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Thomas</t>
+          <t>Yannic</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C17" t="n">
         <v>20</v>
       </c>
       <c r="D17" t="n">
-        <v>41162</v>
+        <v>56704</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>elNhqm</t>
+          <t>eu9GQx4dz</t>
         </is>
       </c>
       <c r="F17" t="n">
@@ -2708,21 +2828,21 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Ole</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C18" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D18" t="n">
-        <v>78155</v>
+        <v>84942</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>eGUÜäpzL2</t>
+          <t>7fOyotEEt0</t>
         </is>
       </c>
       <c r="F18" t="n">
@@ -2732,21 +2852,21 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Christoph</t>
+          <t>Anja</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="C19" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D19" t="n">
-        <v>30075</v>
+        <v>23736</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>rQLmEöSG5</t>
+          <t>w8äaUy</t>
         </is>
       </c>
       <c r="F19" t="n">
@@ -2756,21 +2876,21 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Felix</t>
+          <t>Ingo</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C20" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D20" t="n">
-        <v>60863</v>
+        <v>99782</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>XyIOY</t>
+          <t>OoäJK29</t>
         </is>
       </c>
       <c r="F20" t="n">
@@ -2780,21 +2900,21 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Christoph</t>
+          <t>Nathalie</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="C21" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D21" t="n">
-        <v>29700</v>
+        <v>33759</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>hüMRlFLs</t>
+          <t>XMspnSOhgr</t>
         </is>
       </c>
       <c r="F21" t="n">
@@ -2804,21 +2924,21 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Louise</t>
+          <t>Josefine</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C22" t="n">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D22" t="n">
-        <v>80176</v>
+        <v>40378</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>keN3K</t>
+          <t>AEvhkn</t>
         </is>
       </c>
       <c r="F22" t="n">
@@ -2828,144 +2948,24 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Miriam</t>
+          <t>Thorsten</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C23" t="n">
         <v>20</v>
       </c>
       <c r="D23" t="n">
-        <v>93731</v>
+        <v>51727</v>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>U3ugtgX</t>
+          <t>8zrLbxs</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Dominik</t>
-        </is>
-      </c>
-      <c r="B24" t="n">
-        <v>25</v>
-      </c>
-      <c r="C24" t="n">
-        <v>20</v>
-      </c>
-      <c r="D24" t="n">
-        <v>14920</v>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>kTiowSä</t>
-        </is>
-      </c>
-      <c r="F24" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Beate</t>
-        </is>
-      </c>
-      <c r="B25" t="n">
-        <v>22</v>
-      </c>
-      <c r="C25" t="n">
-        <v>20</v>
-      </c>
-      <c r="D25" t="n">
-        <v>77261</v>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Zum7cj</t>
-        </is>
-      </c>
-      <c r="F25" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Carla</t>
-        </is>
-      </c>
-      <c r="B26" t="n">
-        <v>28</v>
-      </c>
-      <c r="C26" t="n">
-        <v>20</v>
-      </c>
-      <c r="D26" t="n">
-        <v>55981</v>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>vgv0C</t>
-        </is>
-      </c>
-      <c r="F26" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Felix</t>
-        </is>
-      </c>
-      <c r="B27" t="n">
-        <v>26</v>
-      </c>
-      <c r="C27" t="n">
-        <v>20</v>
-      </c>
-      <c r="D27" t="n">
-        <v>18575</v>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>R7awMO</t>
-        </is>
-      </c>
-      <c r="F27" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Natalie</t>
-        </is>
-      </c>
-      <c r="B28" t="n">
-        <v>32</v>
-      </c>
-      <c r="C28" t="n">
-        <v>30</v>
-      </c>
-      <c r="D28" t="n">
-        <v>30200</v>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>owFkobEm0ä</t>
-        </is>
-      </c>
-      <c r="F28" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>